<commit_message>
Fixed the issue where data with only parent isotopologues cause error
Fixed the issue where data with only parent isotopologues cause error
</commit_message>
<xml_diff>
--- a/inst/extdata/CN_Compound_Test.xlsx
+++ b/inst/extdata/CN_Compound_Test.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box\Accucor\Upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangy\OneDrive\Documents\GitHub\AccuCor2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252A5743-C79F-4BF2-81FF-3DA35F7060AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -22,6 +23,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>compoundId</t>
   </si>
@@ -83,12 +87,15 @@
   </si>
   <si>
     <t>non-labeled-serine_1mM_4</t>
+  </si>
+  <si>
+    <t>Serine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -899,24 +906,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="5.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="15" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="16.26953125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -1618,6 +1625,59 @@
       </c>
       <c r="Q13">
         <v>4301074</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>105.093</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>445783904</v>
+      </c>
+      <c r="G14">
+        <v>452330528</v>
+      </c>
+      <c r="H14">
+        <v>460922144</v>
+      </c>
+      <c r="I14">
+        <v>460856768</v>
+      </c>
+      <c r="J14">
+        <v>240814112</v>
+      </c>
+      <c r="K14">
+        <v>238327808</v>
+      </c>
+      <c r="L14">
+        <v>236562352</v>
+      </c>
+      <c r="M14">
+        <v>238082256</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>